<commit_message>
Updated Degradation curves and DC RTE
</commit_message>
<xml_diff>
--- a/src/DC RTE.xlsx
+++ b/src/DC RTE.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://prevalonenergy-my.sharepoint.com/personal/himanshu_prevalonenergy_com/Documents/I drive/Sizing Tool/DeployWithRender/src/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="43" documentId="11_F25DC773A252ABDACC1048B2119E5C9C5BDE58EB" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8FEFA2DC-E534-48B0-81F0-5E796AFE39AF}"/>
+  <xr:revisionPtr revIDLastSave="53" documentId="11_F25DC773A252ABDACC1048B2119E5C9C5BDE58EB" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9CC62337-E0D9-40C8-A9E1-8CD888A92CBB}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -399,7 +399,7 @@
   <dimension ref="A1:G29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -408,8 +408,7 @@
     <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.42578125" customWidth="1"/>
     <col min="4" max="4" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.42578125" customWidth="1"/>
-    <col min="6" max="6" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="7" width="9.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -502,7 +501,7 @@
         <v>0.95289999999999997</v>
       </c>
       <c r="G4" s="1">
-        <v>0.95289999999999997</v>
+        <v>0.953599999999999</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -511,22 +510,22 @@
         <v>1</v>
       </c>
       <c r="B5" s="1">
-        <v>0.93600000000000005</v>
+        <v>0.93514593616264596</v>
       </c>
       <c r="C5" s="1">
-        <v>0.93600000000000005</v>
+        <v>0.93514593616264596</v>
       </c>
       <c r="D5" s="1">
-        <v>0.95199999999999996</v>
+        <v>0.950882771660431</v>
       </c>
       <c r="E5" s="1">
-        <v>0.95199999999999996</v>
+        <v>0.950882771660431</v>
       </c>
       <c r="F5" s="1">
-        <v>0.95199999999999996</v>
+        <v>0.950882771660431</v>
       </c>
       <c r="G5" s="1">
-        <v>0.95199999999999996</v>
+        <v>0.95196377677195498</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -535,22 +534,22 @@
         <v>2</v>
       </c>
       <c r="B6" s="1">
-        <v>0.93500000000000005</v>
+        <v>0.93373223313476605</v>
       </c>
       <c r="C6" s="1">
-        <v>0.93500000000000005</v>
+        <v>0.93373223313476605</v>
       </c>
       <c r="D6" s="1">
-        <v>0.95109999999999995</v>
+        <v>0.94969433141575599</v>
       </c>
       <c r="E6" s="1">
-        <v>0.95109999999999995</v>
+        <v>0.94969433141575599</v>
       </c>
       <c r="F6" s="1">
-        <v>0.95109999999999995</v>
+        <v>0.94969433141575599</v>
       </c>
       <c r="G6" s="1">
-        <v>0.95109999999999995</v>
+        <v>0.950994155345393</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -559,22 +558,22 @@
         <v>3</v>
       </c>
       <c r="B7" s="1">
-        <v>0.93400000000000005</v>
+        <v>0.93228887716482101</v>
       </c>
       <c r="C7" s="1">
-        <v>0.93400000000000005</v>
+        <v>0.93228887716482101</v>
       </c>
       <c r="D7" s="1">
-        <v>0.95040000000000002</v>
+        <v>0.94874183824396097</v>
       </c>
       <c r="E7" s="1">
-        <v>0.95040000000000002</v>
+        <v>0.94874183824396097</v>
       </c>
       <c r="F7" s="1">
-        <v>0.95040000000000002</v>
+        <v>0.94874183824396097</v>
       </c>
       <c r="G7" s="1">
-        <v>0.95040000000000002</v>
+        <v>0.95019089294109405</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -583,22 +582,22 @@
         <v>4</v>
       </c>
       <c r="B8" s="1">
-        <v>0.93300000000000005</v>
+        <v>0.93078427866583802</v>
       </c>
       <c r="C8" s="1">
-        <v>0.93300000000000005</v>
+        <v>0.93078427866583802</v>
       </c>
       <c r="D8" s="1">
-        <v>0.94969999999999999</v>
+        <v>0.94793503295484105</v>
       </c>
       <c r="E8" s="1">
-        <v>0.94969999999999999</v>
+        <v>0.94793503295484105</v>
       </c>
       <c r="F8" s="1">
-        <v>0.94969999999999999</v>
+        <v>0.94793503295484105</v>
       </c>
       <c r="G8" s="1">
-        <v>0.94969999999999999</v>
+        <v>0.94950020462213303</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -607,22 +606,22 @@
         <v>5</v>
       </c>
       <c r="B9" s="1">
-        <v>0.93200000000000005</v>
+        <v>0.92921336979895497</v>
       </c>
       <c r="C9" s="1">
-        <v>0.93200000000000005</v>
+        <v>0.92921336979895497</v>
       </c>
       <c r="D9" s="1">
-        <v>0.94910000000000005</v>
+        <v>0.94724065094697396</v>
       </c>
       <c r="E9" s="1">
-        <v>0.94910000000000005</v>
+        <v>0.94724065094697396</v>
       </c>
       <c r="F9" s="1">
-        <v>0.94910000000000005</v>
+        <v>0.94724065094697396</v>
       </c>
       <c r="G9" s="1">
-        <v>0.94910000000000005</v>
+        <v>0.94888817071072795</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -631,22 +630,22 @@
         <v>6</v>
       </c>
       <c r="B10" s="1">
-        <v>0.93100000000000005</v>
+        <v>0.92758288749328999</v>
       </c>
       <c r="C10" s="1">
-        <v>0.93100000000000005</v>
+        <v>0.92758288749328999</v>
       </c>
       <c r="D10" s="1">
-        <v>0.9486</v>
+        <v>0.94663199691967104</v>
       </c>
       <c r="E10" s="1">
-        <v>0.9486</v>
+        <v>0.94663199691967104</v>
       </c>
       <c r="F10" s="1">
-        <v>0.9486</v>
+        <v>0.94663199691967104</v>
       </c>
       <c r="G10" s="1">
-        <v>0.9486</v>
+        <v>0.948336858272536</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -655,22 +654,22 @@
         <v>7</v>
       </c>
       <c r="B11" s="1">
-        <v>0.92900000000000005</v>
+        <v>0.92589385433776905</v>
       </c>
       <c r="C11" s="1">
-        <v>0.92900000000000005</v>
+        <v>0.92589385433776905</v>
       </c>
       <c r="D11" s="1">
-        <v>0.94810000000000005</v>
+        <v>0.94609368306825403</v>
       </c>
       <c r="E11" s="1">
-        <v>0.94810000000000005</v>
+        <v>0.94609368306825403</v>
       </c>
       <c r="F11" s="1">
-        <v>0.94810000000000005</v>
+        <v>0.94609368306825403</v>
       </c>
       <c r="G11" s="1">
-        <v>0.94810000000000005</v>
+        <v>0.947843862971402</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -679,22 +678,22 @@
         <v>8</v>
       </c>
       <c r="B12" s="1">
-        <v>0.92700000000000005</v>
+        <v>0.92415565467384797</v>
       </c>
       <c r="C12" s="1">
-        <v>0.92700000000000005</v>
+        <v>0.92415565467384797</v>
       </c>
       <c r="D12" s="1">
-        <v>0.9476</v>
+        <v>0.94560735245906402</v>
       </c>
       <c r="E12" s="1">
-        <v>0.9476</v>
+        <v>0.94560735245906402</v>
       </c>
       <c r="F12" s="1">
-        <v>0.9476</v>
+        <v>0.94560735245906402</v>
       </c>
       <c r="G12" s="1">
-        <v>0.9476</v>
+        <v>0.94739077026818697</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -703,22 +702,22 @@
         <v>9</v>
       </c>
       <c r="B13" s="1">
-        <v>0.92600000000000005</v>
+        <v>0.92238272038232005</v>
       </c>
       <c r="C13" s="1">
-        <v>0.92600000000000005</v>
+        <v>0.92238272038232005</v>
       </c>
       <c r="D13" s="1">
-        <v>0.94720000000000004</v>
+        <v>0.94516505311437604</v>
       </c>
       <c r="E13" s="1">
-        <v>0.94720000000000004</v>
+        <v>0.94516505311437604</v>
       </c>
       <c r="F13" s="1">
-        <v>0.94720000000000004</v>
+        <v>0.94516505311437604</v>
       </c>
       <c r="G13" s="1">
-        <v>0.94720000000000004</v>
+        <v>0.94697850254651905</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -727,22 +726,22 @@
         <v>10</v>
       </c>
       <c r="B14" s="1">
-        <v>0.92500000000000004</v>
+        <v>0.92058645543171003</v>
       </c>
       <c r="C14" s="1">
-        <v>0.92500000000000004</v>
+        <v>0.92058645543171003</v>
       </c>
       <c r="D14" s="1">
-        <v>0.94669999999999999</v>
+        <v>0.944755747752416</v>
       </c>
       <c r="E14" s="1">
-        <v>0.94669999999999999</v>
+        <v>0.944755747752416</v>
       </c>
       <c r="F14" s="1">
-        <v>0.94669999999999999</v>
+        <v>0.944755747752416</v>
       </c>
       <c r="G14" s="1">
-        <v>0.94669999999999999</v>
+        <v>0.94659680971226501</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -751,22 +750,22 @@
         <v>11</v>
       </c>
       <c r="B15" s="1">
-        <v>0.92300000000000004</v>
+        <v>0.91876356808079196</v>
       </c>
       <c r="C15" s="1">
-        <v>0.92300000000000004</v>
+        <v>0.91876356808079196</v>
       </c>
       <c r="D15" s="1">
-        <v>0.94630000000000003</v>
+        <v>0.94436603844664202</v>
       </c>
       <c r="E15" s="1">
-        <v>0.94630000000000003</v>
+        <v>0.94436603844664202</v>
       </c>
       <c r="F15" s="1">
-        <v>0.94630000000000003</v>
+        <v>0.94436603844664202</v>
       </c>
       <c r="G15" s="1">
-        <v>0.94630000000000003</v>
+        <v>0.94624277082437902</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -775,22 +774,22 @@
         <v>12</v>
       </c>
       <c r="B16" s="1">
-        <v>0.92100000000000004</v>
+        <v>0.91694270131199995</v>
       </c>
       <c r="C16" s="1">
-        <v>0.92100000000000004</v>
+        <v>0.91694270131199995</v>
       </c>
       <c r="D16" s="1">
-        <v>0.94589999999999996</v>
+        <v>0.94398878474407499</v>
       </c>
       <c r="E16" s="1">
-        <v>0.94589999999999996</v>
+        <v>0.94398878474407499</v>
       </c>
       <c r="F16" s="1">
-        <v>0.94589999999999996</v>
+        <v>0.94398878474407499</v>
       </c>
       <c r="G16" s="1">
-        <v>0.94589999999999996</v>
+        <v>0.94591331998732398</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -799,22 +798,22 @@
         <v>13</v>
       </c>
       <c r="B17" s="1">
-        <v>0.91900000000000004</v>
+        <v>0.91510349559824999</v>
       </c>
       <c r="C17" s="1">
-        <v>0.91900000000000004</v>
+        <v>0.91510349559824999</v>
       </c>
       <c r="D17" s="1">
-        <v>0.9456</v>
+        <v>0.94361704167489402</v>
       </c>
       <c r="E17" s="1">
-        <v>0.9456</v>
+        <v>0.94361704167489402</v>
       </c>
       <c r="F17" s="1">
-        <v>0.9456</v>
+        <v>0.94361704167489402</v>
       </c>
       <c r="G17" s="1">
-        <v>0.9456</v>
+        <v>0.94559924726702205</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -823,22 +822,22 @@
         <v>14</v>
       </c>
       <c r="B18" s="1">
-        <v>0.91700000000000004</v>
+        <v>0.91328459998148703</v>
       </c>
       <c r="C18" s="1">
-        <v>0.91700000000000004</v>
+        <v>0.91328459998148703</v>
       </c>
       <c r="D18" s="1">
-        <v>0.94520000000000004</v>
+        <v>0.94324427329647698</v>
       </c>
       <c r="E18" s="1">
-        <v>0.94520000000000004</v>
+        <v>0.94324427329647698</v>
       </c>
       <c r="F18" s="1">
-        <v>0.94520000000000004</v>
+        <v>0.94324427329647698</v>
       </c>
       <c r="G18" s="1">
-        <v>0.94520000000000004</v>
+        <v>0.94530094826535105</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
@@ -847,22 +846,22 @@
         <v>15</v>
       </c>
       <c r="B19" s="1">
-        <v>0.91500000000000004</v>
+        <v>0.91147450103442296</v>
       </c>
       <c r="C19" s="1">
-        <v>0.91500000000000004</v>
+        <v>0.91147450103442296</v>
       </c>
       <c r="D19" s="1">
-        <v>0.94489999999999996</v>
+        <v>0.94285782645141003</v>
       </c>
       <c r="E19" s="1">
-        <v>0.94489999999999996</v>
+        <v>0.94285782645141003</v>
       </c>
       <c r="F19" s="1">
-        <v>0.94489999999999996</v>
+        <v>0.94285782645141003</v>
       </c>
       <c r="G19" s="1">
-        <v>0.94489999999999996</v>
+        <v>0.94501562908699299</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
@@ -871,22 +870,22 @@
         <v>16</v>
       </c>
       <c r="B20" s="1">
-        <v>0.91300000000000003</v>
+        <v>0.90969842766601605</v>
       </c>
       <c r="C20" s="1">
-        <v>0.91300000000000003</v>
+        <v>0.90969842766601605</v>
       </c>
       <c r="D20" s="1">
-        <v>0.94450000000000001</v>
+        <v>0.94245453834051096</v>
       </c>
       <c r="E20" s="1">
-        <v>0.94450000000000001</v>
+        <v>0.94245453834051096</v>
       </c>
       <c r="F20" s="1">
-        <v>0.94450000000000001</v>
+        <v>0.94245453834051096</v>
       </c>
       <c r="G20" s="1">
-        <v>0.94450000000000001</v>
+        <v>0.94473763747780004</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
@@ -895,22 +894,22 @@
         <v>17</v>
       </c>
       <c r="B21" s="1">
-        <v>0.91100000000000003</v>
+        <v>0.90794240492960898</v>
       </c>
       <c r="C21" s="1">
-        <v>0.91100000000000003</v>
+        <v>0.90794240492960898</v>
       </c>
       <c r="D21" s="1">
-        <v>0.94420000000000004</v>
+        <v>0.94202869950634005</v>
       </c>
       <c r="E21" s="1">
-        <v>0.94420000000000004</v>
+        <v>0.94202869950634005</v>
       </c>
       <c r="F21" s="1">
-        <v>0.94420000000000004</v>
+        <v>0.94202869950634005</v>
       </c>
       <c r="G21" s="1">
-        <v>0.94420000000000004</v>
+        <v>0.94446140514422705</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
@@ -919,22 +918,22 @@
         <v>18</v>
       </c>
       <c r="B22" s="1">
-        <v>0.90900000000000003</v>
+        <v>0.90624330522344798</v>
       </c>
       <c r="C22" s="1">
-        <v>0.90900000000000003</v>
+        <v>0.90624330522344798</v>
       </c>
       <c r="D22" s="1">
-        <v>0.94389999999999996</v>
+        <v>0.94157083965852695</v>
       </c>
       <c r="E22" s="1">
-        <v>0.94389999999999996</v>
+        <v>0.94157083965852695</v>
       </c>
       <c r="F22" s="1">
-        <v>0.94389999999999996</v>
+        <v>0.94157083965852695</v>
       </c>
       <c r="G22" s="1">
-        <v>0.94389999999999996</v>
+        <v>0.94419043568845495</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
@@ -943,22 +942,22 @@
         <v>19</v>
       </c>
       <c r="B23" s="1">
-        <v>0.90700000000000003</v>
+        <v>0.90458583576141005</v>
       </c>
       <c r="C23" s="1">
-        <v>0.90700000000000003</v>
+        <v>0.90458583576141005</v>
       </c>
       <c r="D23" s="1">
-        <v>0.94359999999999999</v>
+        <v>0.94107509372639397</v>
       </c>
       <c r="E23" s="1">
-        <v>0.94359999999999999</v>
+        <v>0.94107509372639397</v>
       </c>
       <c r="F23" s="1">
-        <v>0.94359999999999999</v>
+        <v>0.94107509372639397</v>
       </c>
       <c r="G23" s="1">
-        <v>0.94359999999999999</v>
+        <v>0.94391620689553102</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
@@ -967,22 +966,22 @@
         <v>20</v>
       </c>
       <c r="B24" s="1">
-        <v>0.90500000000000003</v>
+        <v>0.90298021780622295</v>
       </c>
       <c r="C24" s="1">
-        <v>0.90500000000000003</v>
+        <v>0.90298021780622295</v>
       </c>
       <c r="D24" s="1">
-        <v>0.94330000000000003</v>
+        <v>0.940535909879054</v>
       </c>
       <c r="E24" s="1">
-        <v>0.94330000000000003</v>
+        <v>0.940535909879054</v>
       </c>
       <c r="F24" s="1">
-        <v>0.94330000000000003</v>
+        <v>0.940535909879054</v>
       </c>
       <c r="G24" s="1">
-        <v>0.94330000000000003</v>
+        <v>0.943639419103669</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added assumptions to the Tool
</commit_message>
<xml_diff>
--- a/src/DC RTE.xlsx
+++ b/src/DC RTE.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://prevalonenergy-my.sharepoint.com/personal/himanshu_prevalonenergy_com/Documents/I drive/Sizing Tool/DeployWithRender/src/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="53" documentId="11_F25DC773A252ABDACC1048B2119E5C9C5BDE58EB" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9CC62337-E0D9-40C8-A9E1-8CD888A92CBB}"/>
+  <xr:revisionPtr revIDLastSave="54" documentId="11_F25DC773A252ABDACC1048B2119E5C9C5BDE58EB" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EFE44B48-0738-4230-8BB4-5D2DB8626279}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-90" yWindow="0" windowWidth="19380" windowHeight="20970" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -110,11 +110,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -131,6 +132,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -399,19 +404,19 @@
   <dimension ref="A1:G29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+      <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.42578125" customWidth="1"/>
-    <col min="4" max="4" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="7" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.453125" customWidth="1"/>
+    <col min="4" max="4" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="5" max="7" width="9.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -440,7 +445,7 @@
         <v>HD 511 | 8</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
       <c r="B2" s="1" t="s">
         <v>0</v>
@@ -461,7 +466,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B3" s="3">
         <v>2</v>
       </c>
@@ -481,7 +486,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" s="2">
         <v>0</v>
       </c>
@@ -491,7 +496,7 @@
       <c r="C4" s="1">
         <v>0.93700000000000006</v>
       </c>
-      <c r="D4" s="1">
+      <c r="D4" s="4">
         <v>0.95289999999999997</v>
       </c>
       <c r="E4" s="1">
@@ -504,7 +509,7 @@
         <v>0.953599999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" s="2">
         <f>A4+1</f>
         <v>1</v>
@@ -515,7 +520,7 @@
       <c r="C5" s="1">
         <v>0.93514593616264596</v>
       </c>
-      <c r="D5" s="1">
+      <c r="D5" s="4">
         <v>0.950882771660431</v>
       </c>
       <c r="E5" s="1">
@@ -528,7 +533,7 @@
         <v>0.95196377677195498</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" s="2">
         <f t="shared" ref="A6:A29" si="1">A5+1</f>
         <v>2</v>
@@ -539,7 +544,7 @@
       <c r="C6" s="1">
         <v>0.93373223313476605</v>
       </c>
-      <c r="D6" s="1">
+      <c r="D6" s="4">
         <v>0.94969433141575599</v>
       </c>
       <c r="E6" s="1">
@@ -552,7 +557,7 @@
         <v>0.950994155345393</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" s="2">
         <f t="shared" si="1"/>
         <v>3</v>
@@ -563,7 +568,7 @@
       <c r="C7" s="1">
         <v>0.93228887716482101</v>
       </c>
-      <c r="D7" s="1">
+      <c r="D7" s="4">
         <v>0.94874183824396097</v>
       </c>
       <c r="E7" s="1">
@@ -576,7 +581,7 @@
         <v>0.95019089294109405</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" s="2">
         <f t="shared" si="1"/>
         <v>4</v>
@@ -587,7 +592,7 @@
       <c r="C8" s="1">
         <v>0.93078427866583802</v>
       </c>
-      <c r="D8" s="1">
+      <c r="D8" s="4">
         <v>0.94793503295484105</v>
       </c>
       <c r="E8" s="1">
@@ -600,7 +605,7 @@
         <v>0.94950020462213303</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" s="2">
         <f t="shared" si="1"/>
         <v>5</v>
@@ -611,7 +616,7 @@
       <c r="C9" s="1">
         <v>0.92921336979895497</v>
       </c>
-      <c r="D9" s="1">
+      <c r="D9" s="4">
         <v>0.94724065094697396</v>
       </c>
       <c r="E9" s="1">
@@ -624,7 +629,7 @@
         <v>0.94888817071072795</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" s="2">
         <f t="shared" si="1"/>
         <v>6</v>
@@ -635,7 +640,7 @@
       <c r="C10" s="1">
         <v>0.92758288749328999</v>
       </c>
-      <c r="D10" s="1">
+      <c r="D10" s="4">
         <v>0.94663199691967104</v>
       </c>
       <c r="E10" s="1">
@@ -648,7 +653,7 @@
         <v>0.948336858272536</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" s="2">
         <f t="shared" si="1"/>
         <v>7</v>
@@ -659,7 +664,7 @@
       <c r="C11" s="1">
         <v>0.92589385433776905</v>
       </c>
-      <c r="D11" s="1">
+      <c r="D11" s="4">
         <v>0.94609368306825403</v>
       </c>
       <c r="E11" s="1">
@@ -672,7 +677,7 @@
         <v>0.947843862971402</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" s="2">
         <f t="shared" si="1"/>
         <v>8</v>
@@ -683,7 +688,7 @@
       <c r="C12" s="1">
         <v>0.92415565467384797</v>
       </c>
-      <c r="D12" s="1">
+      <c r="D12" s="4">
         <v>0.94560735245906402</v>
       </c>
       <c r="E12" s="1">
@@ -696,7 +701,7 @@
         <v>0.94739077026818697</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" s="2">
         <f t="shared" si="1"/>
         <v>9</v>
@@ -707,7 +712,7 @@
       <c r="C13" s="1">
         <v>0.92238272038232005</v>
       </c>
-      <c r="D13" s="1">
+      <c r="D13" s="4">
         <v>0.94516505311437604</v>
       </c>
       <c r="E13" s="1">
@@ -720,7 +725,7 @@
         <v>0.94697850254651905</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14" s="2">
         <f t="shared" si="1"/>
         <v>10</v>
@@ -731,7 +736,7 @@
       <c r="C14" s="1">
         <v>0.92058645543171003</v>
       </c>
-      <c r="D14" s="1">
+      <c r="D14" s="4">
         <v>0.944755747752416</v>
       </c>
       <c r="E14" s="1">
@@ -744,7 +749,7 @@
         <v>0.94659680971226501</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15" s="2">
         <f t="shared" si="1"/>
         <v>11</v>
@@ -755,7 +760,7 @@
       <c r="C15" s="1">
         <v>0.91876356808079196</v>
       </c>
-      <c r="D15" s="1">
+      <c r="D15" s="4">
         <v>0.94436603844664202</v>
       </c>
       <c r="E15" s="1">
@@ -768,7 +773,7 @@
         <v>0.94624277082437902</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A16" s="2">
         <f t="shared" si="1"/>
         <v>12</v>
@@ -779,7 +784,7 @@
       <c r="C16" s="1">
         <v>0.91694270131199995</v>
       </c>
-      <c r="D16" s="1">
+      <c r="D16" s="4">
         <v>0.94398878474407499</v>
       </c>
       <c r="E16" s="1">
@@ -792,7 +797,7 @@
         <v>0.94591331998732398</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A17" s="2">
         <f t="shared" si="1"/>
         <v>13</v>
@@ -803,7 +808,7 @@
       <c r="C17" s="1">
         <v>0.91510349559824999</v>
       </c>
-      <c r="D17" s="1">
+      <c r="D17" s="4">
         <v>0.94361704167489402</v>
       </c>
       <c r="E17" s="1">
@@ -816,7 +821,7 @@
         <v>0.94559924726702205</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A18" s="2">
         <f t="shared" si="1"/>
         <v>14</v>
@@ -827,7 +832,7 @@
       <c r="C18" s="1">
         <v>0.91328459998148703</v>
       </c>
-      <c r="D18" s="1">
+      <c r="D18" s="4">
         <v>0.94324427329647698</v>
       </c>
       <c r="E18" s="1">
@@ -840,7 +845,7 @@
         <v>0.94530094826535105</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A19" s="2">
         <f t="shared" si="1"/>
         <v>15</v>
@@ -851,7 +856,7 @@
       <c r="C19" s="1">
         <v>0.91147450103442296</v>
       </c>
-      <c r="D19" s="1">
+      <c r="D19" s="4">
         <v>0.94285782645141003</v>
       </c>
       <c r="E19" s="1">
@@ -864,7 +869,7 @@
         <v>0.94501562908699299</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A20" s="2">
         <f t="shared" si="1"/>
         <v>16</v>
@@ -875,7 +880,7 @@
       <c r="C20" s="1">
         <v>0.90969842766601605</v>
       </c>
-      <c r="D20" s="1">
+      <c r="D20" s="4">
         <v>0.94245453834051096</v>
       </c>
       <c r="E20" s="1">
@@ -888,7 +893,7 @@
         <v>0.94473763747780004</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A21" s="2">
         <f t="shared" si="1"/>
         <v>17</v>
@@ -899,7 +904,7 @@
       <c r="C21" s="1">
         <v>0.90794240492960898</v>
       </c>
-      <c r="D21" s="1">
+      <c r="D21" s="4">
         <v>0.94202869950634005</v>
       </c>
       <c r="E21" s="1">
@@ -912,7 +917,7 @@
         <v>0.94446140514422705</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A22" s="2">
         <f t="shared" si="1"/>
         <v>18</v>
@@ -923,7 +928,7 @@
       <c r="C22" s="1">
         <v>0.90624330522344798</v>
       </c>
-      <c r="D22" s="1">
+      <c r="D22" s="4">
         <v>0.94157083965852695</v>
       </c>
       <c r="E22" s="1">
@@ -936,7 +941,7 @@
         <v>0.94419043568845495</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A23" s="2">
         <f t="shared" si="1"/>
         <v>19</v>
@@ -947,7 +952,7 @@
       <c r="C23" s="1">
         <v>0.90458583576141005</v>
       </c>
-      <c r="D23" s="1">
+      <c r="D23" s="4">
         <v>0.94107509372639397</v>
       </c>
       <c r="E23" s="1">
@@ -960,7 +965,7 @@
         <v>0.94391620689553102</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A24" s="2">
         <f t="shared" si="1"/>
         <v>20</v>
@@ -971,7 +976,7 @@
       <c r="C24" s="1">
         <v>0.90298021780622295</v>
       </c>
-      <c r="D24" s="1">
+      <c r="D24" s="4">
         <v>0.940535909879054</v>
       </c>
       <c r="E24" s="1">
@@ -984,7 +989,7 @@
         <v>0.943639419103669</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A25" s="2">
         <f t="shared" si="1"/>
         <v>21</v>
@@ -1008,7 +1013,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A26" s="2">
         <f t="shared" si="1"/>
         <v>22</v>
@@ -1032,7 +1037,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A27" s="2">
         <f t="shared" si="1"/>
         <v>23</v>
@@ -1056,7 +1061,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A28" s="2">
         <f t="shared" si="1"/>
         <v>24</v>
@@ -1080,7 +1085,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A29" s="2">
         <f t="shared" si="1"/>
         <v>25</v>
@@ -1108,4 +1113,10 @@
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
+<clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
+  <clbl:label id="{cb900d8d-e34c-495b-bcac-83a2298b7739}" enabled="1" method="Standard" siteId="{fda0a4a7-3813-444d-808d-54bb327d0367}" removed="0"/>
+</clbl:labelList>
 </file>
</xml_diff>